<commit_message>
updated all excel files to give clear picture
</commit_message>
<xml_diff>
--- a/Hacktoberfest_Expected_Ouputt.xlsx
+++ b/Hacktoberfest_Expected_Ouputt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anshul.choudhary@ibm.com/PycharmProjects/Manipulating_Excel_Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F476D9-5E2B-4745-A3CF-2C38DA12E420}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8071346-3FDB-3E45-9358-098EC194CE4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19340" yWindow="8520" windowWidth="26040" windowHeight="14940" xr2:uid="{240A953C-158B-9649-AC89-6A8615E9C240}"/>
+    <workbookView xWindow="27780" yWindow="6100" windowWidth="26040" windowHeight="14940" xr2:uid="{240A953C-158B-9649-AC89-6A8615E9C240}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Destination</t>
   </si>
@@ -50,12 +50,6 @@
     <t>1.4.3.2</t>
   </si>
   <si>
-    <t>3.3.5.6</t>
-  </si>
-  <si>
-    <t>156.78.90.3</t>
-  </si>
-  <si>
     <t>Source Color</t>
   </si>
   <si>
@@ -71,24 +65,15 @@
     <t>Yellow</t>
   </si>
   <si>
-    <t>Brown</t>
-  </si>
-  <si>
     <t>Grey</t>
   </si>
   <si>
-    <t>5.7.8.9</t>
-  </si>
-  <si>
     <t>fsfgsg</t>
   </si>
   <si>
     <t>gsgs</t>
   </si>
   <si>
-    <t xml:space="preserve">Consider 5 Colors above only </t>
-  </si>
-  <si>
     <t>fsd</t>
   </si>
   <si>
@@ -99,13 +84,6 @@
   </si>
   <si>
     <t>1.2.3.4</t>
-  </si>
-  <si>
-    <t>6.208.46.246,6.208.48.81,
-6.208.48.48</t>
-  </si>
-  <si>
-    <t>6.214.16.167</t>
   </si>
   <si>
     <t>6.208.46.246,
@@ -116,6 +94,28 @@
     <t>6.208.46.0/23
 6.208.48.81
 6.208.48.48</t>
+  </si>
+  <si>
+    <t>1.2.1.12</t>
+  </si>
+  <si>
+    <t>1.2.1.0/24</t>
+  </si>
+  <si>
+    <t>1.2.11.3,1.2.11.5, 1.2.11.5
+1.2.12.1
+1.2.12.4</t>
+  </si>
+  <si>
+    <t>6.208.46.0/23
+6.208.48.81
+1.2.42.3</t>
+  </si>
+  <si>
+    <t>1.2.1.1,1.2.1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consider 4 Colors above only </t>
   </si>
 </sst>
 </file>
@@ -170,12 +170,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA58034"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -189,6 +183,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -214,7 +214,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -222,6 +221,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -546,7 +548,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,16 +561,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>
@@ -584,73 +586,73 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>24</v>
+      <c r="F6" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -660,7 +662,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added more support lines
</commit_message>
<xml_diff>
--- a/Hacktoberfest_Expected_Ouputt.xlsx
+++ b/Hacktoberfest_Expected_Ouputt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anshul.choudhary@ibm.com/PycharmProjects/Manipulating_Excel_Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D240215F-5AB0-9E4F-96B6-C80CA54A8E57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E9A100-44AE-BB4D-85DB-C134A7DC6E47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{240A953C-158B-9649-AC89-6A8615E9C240}"/>
+    <workbookView xWindow="17620" yWindow="6100" windowWidth="33580" windowHeight="18960" xr2:uid="{240A953C-158B-9649-AC89-6A8615E9C240}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Destination</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Deny</t>
+  </si>
+  <si>
+    <t>#output based on sheet1 of Hacktoberfest_database.xlsx</t>
   </si>
 </sst>
 </file>
@@ -622,12 +625,12 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="1" max="1" width="52.1640625" customWidth="1"/>
     <col min="2" max="2" width="24.83203125" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="6" max="6" width="35.1640625" customWidth="1"/>
@@ -792,6 +795,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>24</v>

</xml_diff>